<commit_message>
update result 20201123 & update plan 20201124
</commit_message>
<xml_diff>
--- a/20201123.xlsx
+++ b/20201123.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9145CCC-0B50-4774-A1D4-20D3677C4283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746F5D9E-5E27-48D5-BB94-C39FCFA225E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>일</t>
   </si>
@@ -138,10 +138,6 @@
   </si>
   <si>
     <t>할 일</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>사유</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
@@ -214,7 +210,31 @@
     <t>1. 2채널
  - 온도이슈
   -&gt; 온도가 실제온도보다 약 4~5도 낮게 나오는 현상
-   =&gt; ADC시작전 calibaration함수 실행</t>
+   =&gt; ADC시작전 calibaration함수 실행
+ - 생산
+  -&gt; 100ea 라이팅 및 온도테스트 완료
+2. 모빌리티
+ - 멀티 NCT연결 시 connect가 됬다 안됬다 하는 현상
+  -&gt; Mac충돌로 인한 경우임, Mac을 서로 다르게 사용
+ - e1전문 변경
+  -&gt; e1전문의 시작시간 부분을 현재 rtc시간이 아닌 CT에서 주는 1바이트만 적용
+   =&gt; 나머지 바이트는 0으로 초기화
+ - 재연결 관련 이슈 검토
+  -&gt; disconnect 시 약 27초의 판단시간 필요.
+   =&gt; DHCP쓰지 않을 경우는 2~3초 내에 판단가능 하나, 쓸 경우는 안됨
+    ==&gt; 기존 F7에 사용하였던 packet timeout api가 적용이 안되는 듯?</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>늦잠</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>정체… 넘어렵다..</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 어항 물 갈기</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -388,7 +408,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,18 +598,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -601,12 +609,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -736,6 +762,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -871,84 +934,81 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1483,7 +1543,7 @@
   <dimension ref="B2:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E3" sqref="E3:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1508,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>30</v>
@@ -1519,7 +1579,7 @@
       <c r="G2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="4"/>
       <c r="I2" t="s">
         <v>15</v>
       </c>
@@ -1537,21 +1597,25 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="18" t="s">
+      <c r="B3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="25"/>
+      <c r="E3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="G3" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="H3" s="4"/>
       <c r="I3" t="s">
         <v>13</v>
       </c>
@@ -1563,13 +1627,13 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="25"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="8"/>
+      <c r="H4" s="4"/>
       <c r="I4" t="s">
         <v>11</v>
       </c>
@@ -1578,13 +1642,13 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="20"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="15"/>
-      <c r="H5" s="8"/>
+      <c r="H5" s="4"/>
       <c r="I5" t="s">
         <v>12</v>
       </c>
@@ -1593,13 +1657,13 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="25"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="8"/>
+      <c r="H6" s="4"/>
       <c r="I6" t="s">
         <v>10</v>
       </c>
@@ -1608,13 +1672,13 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="20"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="8"/>
+      <c r="H7" s="4"/>
       <c r="I7" t="s">
         <v>8</v>
       </c>
@@ -1627,13 +1691,13 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="20"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="25"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="14"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="8"/>
+      <c r="H8" s="4"/>
       <c r="I8" t="s">
         <v>4</v>
       </c>
@@ -1642,199 +1706,201 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
+      <c r="D10" s="19"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="19"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
+      <c r="D19" s="19"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="19"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="9" t="s">
+      <c r="C23" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="25"/>
+      <c r="D23" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="17"/>
-      <c r="H23" s="8"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
@@ -1846,9 +1912,9 @@
     <mergeCell ref="E3:E23"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
-    <mergeCell ref="D3:D8"/>
     <mergeCell ref="F3:F14"/>
     <mergeCell ref="F15:F23"/>
+    <mergeCell ref="D3:D9"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>